<commit_message>
Update manual_curation.xlsx to only show examples #11
</commit_message>
<xml_diff>
--- a/data/manual_curation.xlsx
+++ b/data/manual_curation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/refinegems/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F2260A-7794-134E-B784-1CA205B4C966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939E5CFF-60B0-9944-A0C2-9E638040F82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metab" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>BIGG</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>sbo</t>
+  </si>
+  <si>
+    <t>examples</t>
   </si>
 </sst>
 </file>
@@ -589,9 +592,9 @@
   </sheetPr>
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K88" sqref="A82:K88"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -676,7 +679,9 @@
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1933,7 +1938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35DF402-707E-F145-925A-05F806C63C3A}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>